<commit_message>
Commiting code that gets test data from excel files
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Data.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Data.xlsx
@@ -2,19 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Language" sheetId="1" r:id="rId1"/>
+    <sheet name="Skill" sheetId="2" r:id="rId1"/>
+    <sheet name="Education" sheetId="3" r:id="rId2"/>
+    <sheet name="Certification" sheetId="4" r:id="rId3"/>
+    <sheet name="Language" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Language</t>
   </si>
@@ -35,12 +38,63 @@
   </si>
   <si>
     <t>Korean</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Skill1</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>AUT</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Institute</t>
+  </si>
+  <si>
+    <t>Associate</t>
+  </si>
+  <si>
+    <t>Test Analyst</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Certificate</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Certified Tester Foundation Level</t>
+  </si>
+  <si>
+    <t>ISTQB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,10 +431,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>2022</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>2022</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>